<commit_message>
Fix blank import fields: cost_impact, review_comments, maintenance dates, user lookup
- RFIs: add cost_impact, schedule_impact_days, answer, assigned_to to import handlers
- Submittals: add reviewer_id (via user lookup), review_comments to import handlers
- Maintenance: add actual_cost, notes, assigned_to to import handlers
- Equipment: add last_maintenance_date, next_maintenance_date to import handlers
- Equipment Maintenance: backfill equipment dates after importing maintenance logs
- Add shared user profile name-to-UUID lookup for assigned_to/reviewer FK fields
- Update import-config.ts with new columns for RFIs, Submittals, Equipment, Maintenance
- Update mock data CSVs and template headers with new columns
- Rebuild master xlsx (30 sheets, 624 rows)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/mock-data/New/MERIDIAN_DEV_GROUP_MASTER_TEST/Meridian_Development_Group_Master.xlsx
+++ b/mock-data/New/MERIDIAN_DEV_GROUP_MASTER_TEST/Meridian_Development_Group_Master.xlsx
@@ -6778,7 +6778,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6802,6 +6802,12 @@
       <c r="F1" t="str">
         <v>project_name</v>
       </c>
+      <c r="G1" t="str">
+        <v>cost_impact</v>
+      </c>
+      <c r="H1" t="str">
+        <v>schedule_impact_days</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -6822,6 +6828,12 @@
       <c r="F2" t="str">
         <v>Downtown Convention Center</v>
       </c>
+      <c r="G2" t="str">
+        <v>12500</v>
+      </c>
+      <c r="H2" t="str">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -6842,6 +6854,12 @@
       <c r="F3" t="str">
         <v>Downtown Convention Center</v>
       </c>
+      <c r="G3" t="str">
+        <v>8200</v>
+      </c>
+      <c r="H3" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -6862,6 +6880,12 @@
       <c r="F4" t="str">
         <v>Downtown Convention Center</v>
       </c>
+      <c r="G4" t="str">
+        <v>35000</v>
+      </c>
+      <c r="H4" t="str">
+        <v>7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -6882,6 +6906,12 @@
       <c r="F5" t="str">
         <v>Downtown Convention Center</v>
       </c>
+      <c r="G5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -6902,6 +6932,12 @@
       <c r="F6" t="str">
         <v>Downtown Convention Center</v>
       </c>
+      <c r="G6" t="str">
+        <v>15000</v>
+      </c>
+      <c r="H6" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -6922,6 +6958,12 @@
       <c r="F7" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
+      <c r="G7" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -6942,6 +6984,12 @@
       <c r="F8" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
+      <c r="G8" t="str">
+        <v>22000</v>
+      </c>
+      <c r="H8" t="str">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -6962,6 +7010,12 @@
       <c r="F9" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
+      <c r="G9" t="str">
+        <v>18500</v>
+      </c>
+      <c r="H9" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -6982,6 +7036,12 @@
       <c r="F10" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
+      <c r="G10" t="str">
+        <v>6800</v>
+      </c>
+      <c r="H10" t="str">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -7002,6 +7062,12 @@
       <c r="F11" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
+      <c r="G11" t="str">
+        <v>4200</v>
+      </c>
+      <c r="H11" t="str">
+        <v>3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -7022,6 +7088,12 @@
       <c r="F12" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
+      <c r="G12" t="str">
+        <v>2100</v>
+      </c>
+      <c r="H12" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -7042,6 +7114,12 @@
       <c r="F13" t="str">
         <v>Meridian Medical Center</v>
       </c>
+      <c r="G13" t="str">
+        <v>8500</v>
+      </c>
+      <c r="H13" t="str">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -7062,6 +7140,12 @@
       <c r="F14" t="str">
         <v>Meridian Medical Center</v>
       </c>
+      <c r="G14" t="str">
+        <v>12000</v>
+      </c>
+      <c r="H14" t="str">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -7082,6 +7166,12 @@
       <c r="F15" t="str">
         <v>Meridian Medical Center</v>
       </c>
+      <c r="G15" t="str">
+        <v>9800</v>
+      </c>
+      <c r="H15" t="str">
+        <v>3</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -7102,6 +7192,12 @@
       <c r="F16" t="str">
         <v>Shoreline Residences Phase I</v>
       </c>
+      <c r="G16" t="str">
+        <v>3500</v>
+      </c>
+      <c r="H16" t="str">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -7122,10 +7218,16 @@
       <c r="F17" t="str">
         <v>Shoreline Residences Phase I</v>
       </c>
+      <c r="G17" t="str">
+        <v>5600</v>
+      </c>
+      <c r="H17" t="str">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7445,405 +7547,543 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>submittal_number</v>
+      </c>
+      <c r="B1" t="str">
         <v>title</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>project_name</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>spec_section</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>due_date</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>status</v>
+      </c>
+      <c r="G1" t="str">
+        <v>review_comments</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>SUB-001</v>
+      </c>
+      <c r="B2" t="str">
         <v>Structural Steel Shop Drawings</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <v>05 12 00</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>2024-12-01</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>approved</v>
+      </c>
+      <c r="G2" t="str">
+        <v>Approved with comments - verify connection details at moment frame locations per structural addendum 3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>SUB-002</v>
+      </c>
+      <c r="B3" t="str">
         <v>Curtain Wall System</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D3" t="str">
         <v>08 44 13</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <v>2025-06-15</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>approved</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Approved - mockup test passed. Proceed with fabrication per approved sample</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>SUB-003</v>
+      </c>
+      <c r="B4" t="str">
         <v>HVAC Equipment Schedule</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D4" t="str">
         <v>23 00 00</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4" t="str">
         <v>2025-08-01</v>
       </c>
-      <c r="E4" t="str">
+      <c r="F4" t="str">
         <v>approved</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Approved - equipment selections meet spec requirements. Verify electrical connections with Division 26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>SUB-004</v>
+      </c>
+      <c r="B5" t="str">
         <v>Electrical Switchgear</v>
       </c>
-      <c r="B5" t="str">
+      <c r="C5" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D5" t="str">
         <v>26 24 16</v>
       </c>
-      <c r="D5" t="str">
+      <c r="E5" t="str">
         <v>2025-09-01</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <v>approved</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Approved as noted - confirm arc flash labeling per NFPA 70E</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>SUB-005</v>
+      </c>
+      <c r="B6" t="str">
         <v>Elevator Equipment</v>
       </c>
-      <c r="B6" t="str">
+      <c r="C6" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C6" t="str">
+      <c r="D6" t="str">
         <v>14 20 00</v>
       </c>
-      <c r="D6" t="str">
+      <c r="E6" t="str">
         <v>2025-10-15</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <v>pending</v>
+      </c>
+      <c r="G6" t="str">
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>SUB-006</v>
+      </c>
+      <c r="B7" t="str">
         <v>Fire Alarm System</v>
       </c>
-      <c r="B7" t="str">
+      <c r="C7" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C7" t="str">
+      <c r="D7" t="str">
         <v>28 31 00</v>
       </c>
-      <c r="D7" t="str">
+      <c r="E7" t="str">
         <v>2025-11-01</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <v>pending</v>
+      </c>
+      <c r="G7" t="str">
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>SUB-007</v>
+      </c>
+      <c r="B8" t="str">
         <v>Acoustical Ceiling Tiles</v>
       </c>
-      <c r="B8" t="str">
+      <c r="C8" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C8" t="str">
+      <c r="D8" t="str">
         <v>09 51 00</v>
       </c>
-      <c r="D8" t="str">
+      <c r="E8" t="str">
         <v>2026-01-15</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <v>pending</v>
+      </c>
+      <c r="G8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
+        <v>SUB-008</v>
+      </c>
+      <c r="B9" t="str">
         <v>AV System Design</v>
       </c>
-      <c r="B9" t="str">
+      <c r="C9" t="str">
         <v>Downtown Convention Center</v>
       </c>
-      <c r="C9" t="str">
+      <c r="D9" t="str">
         <v>27 41 00</v>
       </c>
-      <c r="D9" t="str">
+      <c r="E9" t="str">
         <v>2026-03-01</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <v>pending</v>
+      </c>
+      <c r="G9" t="str">
+        <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
+        <v>SUB-009</v>
+      </c>
+      <c r="B10" t="str">
         <v>Steel H-Piles</v>
       </c>
-      <c r="B10" t="str">
+      <c r="C10" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
-      <c r="C10" t="str">
+      <c r="D10" t="str">
         <v>31 62 00</v>
       </c>
-      <c r="D10" t="str">
+      <c r="E10" t="str">
         <v>2025-05-15</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <v>approved</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Approved - mill certificates provided. Pile driving contractor to submit driving criteria separately</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
+        <v>SUB-010</v>
+      </c>
+      <c r="B11" t="str">
         <v>Marine Concrete Mix Design</v>
       </c>
-      <c r="B11" t="str">
+      <c r="C11" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
-      <c r="C11" t="str">
+      <c r="D11" t="str">
         <v>03 30 00</v>
       </c>
-      <c r="D11" t="str">
+      <c r="E11" t="str">
         <v>2025-06-01</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <v>approved</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Approved with conditions - maintain 28-day cylinder break results above 6000 PSI</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>SUB-011</v>
+      </c>
+      <c r="B12" t="str">
         <v>Waterproofing Membrane</v>
       </c>
-      <c r="B12" t="str">
+      <c r="C12" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
-      <c r="C12" t="str">
+      <c r="D12" t="str">
         <v>07 10 00</v>
       </c>
-      <c r="D12" t="str">
+      <c r="E12" t="str">
         <v>2025-12-01</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <v>pending</v>
+      </c>
+      <c r="G12" t="str">
+        <v/>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
+        <v>SUB-012</v>
+      </c>
+      <c r="B13" t="str">
         <v>Curtain Wall Mockup</v>
       </c>
-      <c r="B13" t="str">
+      <c r="C13" t="str">
         <v>Waterfront Mixed-Use Tower</v>
       </c>
-      <c r="C13" t="str">
+      <c r="D13" t="str">
         <v>08 44 13</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <v>2026-09-01</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <v>pending</v>
+      </c>
+      <c r="G13" t="str">
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
+        <v>SUB-013</v>
+      </c>
+      <c r="B14" t="str">
         <v>Bridge Bearings</v>
       </c>
-      <c r="B14" t="str">
+      <c r="C14" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
-      <c r="C14" t="str">
+      <c r="D14" t="str">
         <v>34 41 16</v>
       </c>
-      <c r="D14" t="str">
+      <c r="E14" t="str">
         <v>2020-07-01</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <v>approved</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Approved - bearing capacity and movement range verified by structural engineer</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
+        <v>SUB-014</v>
+      </c>
+      <c r="B15" t="str">
         <v>Structural Steel Girders</v>
       </c>
-      <c r="B15" t="str">
+      <c r="C15" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
-      <c r="C15" t="str">
+      <c r="D15" t="str">
         <v>05 12 23</v>
       </c>
-      <c r="D15" t="str">
+      <c r="E15" t="str">
         <v>2020-10-15</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <v>approved</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Approved as submitted</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
+        <v>SUB-015</v>
+      </c>
+      <c r="B16" t="str">
         <v>High Performance Concrete Mix</v>
       </c>
-      <c r="B16" t="str">
+      <c r="C16" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
-      <c r="C16" t="str">
+      <c r="D16" t="str">
         <v>03 31 00</v>
       </c>
-      <c r="D16" t="str">
+      <c r="E16" t="str">
         <v>2021-08-01</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <v>approved</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Approved - HPC mix meets AASHTO requirements for bridge deck application</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v>SUB-016</v>
+      </c>
+      <c r="B17" t="str">
         <v>Seismic Retrofit Hardware</v>
       </c>
-      <c r="B17" t="str">
+      <c r="C17" t="str">
         <v>Highway Bridge Rehabilitation</v>
       </c>
-      <c r="C17" t="str">
+      <c r="D17" t="str">
         <v>05 05 23</v>
       </c>
-      <c r="D17" t="str">
+      <c r="E17" t="str">
         <v>2021-04-15</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <v>approved</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Approved with note - torque values per manufacturer ICC-ES report</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
+        <v>SUB-017</v>
+      </c>
+      <c r="B18" t="str">
         <v>MRI Equipment Specifications</v>
       </c>
-      <c r="B18" t="str">
+      <c r="C18" t="str">
         <v>Meridian Medical Center</v>
       </c>
-      <c r="C18" t="str">
+      <c r="D18" t="str">
         <v>11 52 13</v>
       </c>
-      <c r="D18" t="str">
+      <c r="E18" t="str">
         <v>2023-01-15</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <v>approved</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Approved - RF shielding and vibration isolation requirements confirmed with vendor</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
+        <v>SUB-018</v>
+      </c>
+      <c r="B19" t="str">
         <v>Medical Gas Piping</v>
       </c>
-      <c r="B19" t="str">
+      <c r="C19" t="str">
         <v>Meridian Medical Center</v>
       </c>
-      <c r="C19" t="str">
+      <c r="D19" t="str">
         <v>22 63 00</v>
       </c>
-      <c r="D19" t="str">
+      <c r="E19" t="str">
         <v>2022-06-01</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <v>approved</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Approved - Type K copper per RFI clarification. ASSE 6010 certification required for installer</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
+        <v>SUB-019</v>
+      </c>
+      <c r="B20" t="str">
         <v>Generator and ATS</v>
       </c>
-      <c r="B20" t="str">
+      <c r="C20" t="str">
         <v>Meridian Medical Center</v>
       </c>
-      <c r="C20" t="str">
+      <c r="D20" t="str">
         <v>26 32 13</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <v>2022-04-15</v>
       </c>
-      <c r="E20" t="str">
+      <c r="F20" t="str">
         <v>approved</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Approved - NEC 700 and NFPA 110 compliance verified</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
+        <v>SUB-020</v>
+      </c>
+      <c r="B21" t="str">
         <v>Impact Rated Windows</v>
       </c>
-      <c r="B21" t="str">
+      <c r="C21" t="str">
         <v>Shoreline Residences Phase I</v>
       </c>
-      <c r="C21" t="str">
+      <c r="D21" t="str">
         <v>08 52 00</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <v>2022-11-01</v>
       </c>
-      <c r="E21" t="str">
+      <c r="F21" t="str">
         <v>approved</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Approved - Florida Building Code NOA documentation provided</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
+        <v>SUB-021</v>
+      </c>
+      <c r="B22" t="str">
         <v>Precast Concrete Panels</v>
       </c>
-      <c r="B22" t="str">
+      <c r="C22" t="str">
         <v>Shoreline Residences Phase I</v>
       </c>
-      <c r="C22" t="str">
+      <c r="D22" t="str">
         <v>03 41 00</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <v>2022-09-15</v>
       </c>
-      <c r="E22" t="str">
+      <c r="F22" t="str">
         <v>approved</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Approved with comments - verify panel connection hardware per structural detail SD-12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
+        <v>SUB-022</v>
+      </c>
+      <c r="B23" t="str">
         <v>Pool Mechanical Equipment</v>
       </c>
-      <c r="B23" t="str">
+      <c r="C23" t="str">
         <v>Shoreline Residences Phase I</v>
       </c>
-      <c r="C23" t="str">
+      <c r="D23" t="str">
         <v>13 15 00</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <v>2023-08-01</v>
       </c>
-      <c r="E23" t="str">
+      <c r="F23" t="str">
         <v>approved</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Approved - health department flow rate requirements met</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G23"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -13760,7 +14000,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -13790,6 +14030,12 @@
       <c r="H1" t="str">
         <v>status</v>
       </c>
+      <c r="I1" t="str">
+        <v>actual_cost</v>
+      </c>
+      <c r="J1" t="str">
+        <v>notes</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -13816,6 +14062,12 @@
       <c r="H2" t="str">
         <v>completed</v>
       </c>
+      <c r="I2" t="str">
+        <v>4200</v>
+      </c>
+      <c r="J2" t="str">
+        <v>Compressor replaced same day. Tenant satisfied with response time.</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -13842,6 +14094,12 @@
       <c r="H3" t="str">
         <v>scheduled</v>
       </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v>Weekend work required to minimize tenant impact.</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -13868,6 +14126,12 @@
       <c r="H4" t="str">
         <v>scheduled</v>
       </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v>Coordinate with elevator vendor for after-hours access.</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -13894,6 +14158,12 @@
       <c r="H5" t="str">
         <v>completed</v>
       </c>
+      <c r="I5" t="str">
+        <v>3100</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Upgraded to heat pump model. Slight cost increase but better long-term efficiency.</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -13920,6 +14190,12 @@
       <c r="H6" t="str">
         <v>completed</v>
       </c>
+      <c r="I6" t="str">
+        <v>1850</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Motor replaced and pool reopened within 48 hours.</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -13946,6 +14222,12 @@
       <c r="H7" t="str">
         <v>in_progress</v>
       </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v>Roofer identified failed flashing at parapet wall. Temporary repair in place.</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -13972,6 +14254,12 @@
       <c r="H8" t="str">
         <v>completed</v>
       </c>
+      <c r="I8" t="str">
+        <v>850</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Grease trap cleaned and certified. Next service due October 2025.</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -13998,6 +14286,12 @@
       <c r="H9" t="str">
         <v>scheduled</v>
       </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v>Glass on order. 3-week lead time from manufacturer.</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -14024,6 +14318,12 @@
       <c r="H10" t="str">
         <v>completed</v>
       </c>
+      <c r="I10" t="str">
+        <v>1450</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Repaired and operational. Recommended preventive service for all 6 bay doors.</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -14050,10 +14350,16 @@
       <c r="H11" t="str">
         <v>scheduled</v>
       </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v>Schedule with fire protection contractor. Must complete before insurance renewal.</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -16295,7 +16601,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -16328,6 +16634,12 @@
       <c r="I1" t="str">
         <v>purchase_date</v>
       </c>
+      <c r="J1" t="str">
+        <v>last_maintenance_date</v>
+      </c>
+      <c r="K1" t="str">
+        <v>next_maintenance_date</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -16357,6 +16669,12 @@
       <c r="I2" t="str">
         <v>2019-06-15</v>
       </c>
+      <c r="J2" t="str">
+        <v>2025-02-10</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2025-08-10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -16386,6 +16704,12 @@
       <c r="I3" t="str">
         <v>2020-02-01</v>
       </c>
+      <c r="J3" t="str">
+        <v>2025-01-20</v>
+      </c>
+      <c r="K3" t="str">
+        <v>2026-01-20</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -16415,6 +16739,12 @@
       <c r="I4" t="str">
         <v>2018-09-20</v>
       </c>
+      <c r="J4" t="str">
+        <v>2025-04-10</v>
+      </c>
+      <c r="K4" t="str">
+        <v>2026-04-10</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -16444,6 +16774,12 @@
       <c r="I5" t="str">
         <v>2021-03-10</v>
       </c>
+      <c r="J5" t="str">
+        <v>2025-06-22</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2025-12-22</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -16473,6 +16809,12 @@
       <c r="I6" t="str">
         <v>2022-01-15</v>
       </c>
+      <c r="J6" t="str">
+        <v>2025-09-01</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-01-01</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -16502,6 +16844,12 @@
       <c r="I7" t="str">
         <v>2019-11-01</v>
       </c>
+      <c r="J7" t="str">
+        <v>2025-03-01</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2025-09-01</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -16531,6 +16879,12 @@
       <c r="I8" t="str">
         <v>2020-07-22</v>
       </c>
+      <c r="J8" t="str">
+        <v>2025-03-15</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2025-09-15</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -16560,6 +16914,12 @@
       <c r="I9" t="str">
         <v>2021-05-01</v>
       </c>
+      <c r="J9" t="str">
+        <v>2025-05-01</v>
+      </c>
+      <c r="K9" t="str">
+        <v>2025-08-01</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -16589,6 +16949,12 @@
       <c r="I10" t="str">
         <v>2021-05-01</v>
       </c>
+      <c r="J10" t="str">
+        <v>2025-07-10</v>
+      </c>
+      <c r="K10" t="str">
+        <v>2026-07-10</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -16618,6 +16984,12 @@
       <c r="I11" t="str">
         <v>2021-08-15</v>
       </c>
+      <c r="J11" t="str">
+        <v>2025-04-28</v>
+      </c>
+      <c r="K11" t="str">
+        <v>2025-10-28</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -16647,6 +17019,12 @@
       <c r="I12" t="str">
         <v>2020-04-10</v>
       </c>
+      <c r="J12" t="str">
+        <v>2025-06-15</v>
+      </c>
+      <c r="K12" t="str">
+        <v>2026-06-15</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -16676,10 +17054,16 @@
       <c r="I13" t="str">
         <v>2022-03-20</v>
       </c>
+      <c r="J13" t="str">
+        <v>2025-08-20</v>
+      </c>
+      <c r="K13" t="str">
+        <v>2026-08-20</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K13"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>